<commit_message>
fix: converting to float by mistake when underlines("_") in string
</commit_message>
<xml_diff>
--- a/配置表test/fortest.xlsx
+++ b/配置表test/fortest.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eyewind/someproj/x2j/配置表test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B811281C-EC9C-8C4F-915F-D8D6E0A7BDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D642FA18-4E7C-8F41-A033-D7B154EAE509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3080" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{7C7F3F73-D698-CD4F-B4B7-263B8D60622A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{7C7F3F73-D698-CD4F-B4B7-263B8D60622A}"/>
   </bookViews>
   <sheets>
     <sheet name="#NoKey|测试类型用" sheetId="1" r:id="rId1"/>
-    <sheet name="#ByKey|测试模板" sheetId="3" r:id="rId2"/>
-    <sheet name="#ByGroup|测试模板" sheetId="4" r:id="rId3"/>
-    <sheet name="^WithGroup|测试模板" sheetId="6" r:id="rId4"/>
+    <sheet name="^WithGroup|测试模板" sheetId="6" r:id="rId2"/>
+    <sheet name="#ByKey_测试模板" sheetId="3" r:id="rId3"/>
+    <sheet name="#ByGroup_测试模板" sheetId="4" r:id="rId4"/>
+    <sheet name="#TestFloat|测试float类型" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="69">
   <si>
     <t>1,a,0.5</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -259,6 +260,51 @@
   </si>
   <si>
     <t>^groups</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_float1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_float2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_float3</t>
+  </si>
+  <si>
+    <t>test_float4</t>
+  </si>
+  <si>
+    <t>test_float5</t>
+  </si>
+  <si>
+    <t>test_float6</t>
+  </si>
+  <si>
+    <t>test_float7</t>
+  </si>
+  <si>
+    <t>test_float8</t>
+  </si>
+  <si>
+    <t>test_float9</t>
+  </si>
+  <si>
+    <t>test_float0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>399999999.9996</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>12_34,56_78</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -367,7 +413,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -705,15 +751,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11100240-CD00-D745-830C-14A47A5E1CFF}">
-  <dimension ref="A1:AG13"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:33" ht="16">
+    <row r="1" spans="1:24" ht="16">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="4"/>
@@ -738,17 +784,8 @@
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-    </row>
-    <row r="2" spans="1:33" ht="17">
+    </row>
+    <row r="2" spans="1:24" ht="17">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
@@ -801,10 +838,10 @@
         <v>39</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>39</v>
@@ -821,35 +858,8 @@
       <c r="X2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" ht="17">
+    </row>
+    <row r="3" spans="1:24" ht="17">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -900,7 +910,7 @@
         <v>24</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>24</v>
@@ -920,35 +930,8 @@
       <c r="X3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Y3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" ht="17">
+    </row>
+    <row r="4" spans="1:24" ht="17">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="4"/>
@@ -977,17 +960,8 @@
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-    </row>
-    <row r="5" spans="1:33" ht="17">
+    </row>
+    <row r="5" spans="1:24" ht="17">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1014,45 +988,27 @@
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="4"/>
-    </row>
-    <row r="6" spans="1:33" ht="32">
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6">
         <f t="shared" ref="A6:A13" si="0">ROW()+100</f>
         <v>106</v>
       </c>
-      <c r="C6">
-        <v>123</v>
-      </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" t="s">
+        <v>68</v>
       </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" ht="51">
+    </row>
+    <row r="7" spans="1:24" ht="51">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>107</v>
@@ -1061,13 +1017,16 @@
         <v>-456</v>
       </c>
       <c r="D7">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1076,19 +1035,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:24">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
+      <c r="C8">
+        <v>123</v>
+      </c>
       <c r="D8">
-        <v>1.5</v>
+        <v>-1</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>1</v>
@@ -1098,7 +1060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:24" ht="32">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>109</v>
@@ -1107,13 +1069,28 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>-1.5</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" ht="34">
+        <v>1.5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="34">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>110</v>
@@ -1122,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
@@ -1135,7 +1112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="51">
+    <row r="11" spans="1:24" ht="51">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>111</v>
@@ -1154,7 +1131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:24">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>112</v>
@@ -1176,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:24">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>113</v>
@@ -1199,584 +1176,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7900F381-FBD4-904E-B5C4-BB7E42F8BC8D}">
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:13" ht="16">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" ht="17">
-      <c r="A2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="17">
-      <c r="A3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="17">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" ht="17">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" ht="32">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6">
-        <v>123</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="51">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7">
-        <v>-456</v>
-      </c>
-      <c r="D7">
-        <v>-1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8">
-        <v>123</v>
-      </c>
-      <c r="D8">
-        <v>1.5</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9">
-        <v>123.45</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>-1.5</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A08AD9-4F99-564F-989F-27A8D51E164F}">
-  <dimension ref="A1:M13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:13" ht="16">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" ht="17">
-      <c r="A2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="17">
-      <c r="A3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="17">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" ht="17">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" ht="32">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="51">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>-1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8">
-        <v>123</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1.5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9">
-        <v>123.45</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>-1.5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="32">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="51">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>-1</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12">
-        <v>123</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>1.5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13">
-        <v>123.45</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>-1.5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85038342-107C-654E-B0C2-7D8BB6291F74}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2075,14 +1479,13 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="51">
-      <c r="C11" s="6"/>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11">
         <v>-1</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" t="s">
         <v>51</v>
       </c>
       <c r="I11">
@@ -2135,6 +1538,1096 @@
       </c>
       <c r="J13" s="1">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7900F381-FBD4-904E-B5C4-BB7E42F8BC8D}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="17">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17">
+      <c r="A3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" ht="17">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" ht="32">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>123</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="51">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>-456</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>123</v>
+      </c>
+      <c r="D8">
+        <v>1.5</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>123.45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>-1.5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A08AD9-4F99-564F-989F-27A8D51E164F}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="17">
+      <c r="A2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17">
+      <c r="A3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" ht="17">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" ht="32">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="51">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>123</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1.5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>123.45</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>-1.5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="32">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="51">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12">
+        <v>123</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>1.5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13">
+        <v>123.45</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>-1.5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF282AE9-557B-0849-A0E1-5110EE9E0906}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" customWidth="1"/>
+    <col min="12" max="12" width="36.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" ht="17">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" ht="17">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4">
+        <v>7</v>
+      </c>
+      <c r="I5" s="4">
+        <v>9</v>
+      </c>
+      <c r="J5" s="4">
+        <v>11</v>
+      </c>
+      <c r="K5" s="4">
+        <v>13</v>
+      </c>
+      <c r="L5" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <f t="shared" ref="A6:A13" si="0">ROW()+100</f>
+        <v>106</v>
+      </c>
+      <c r="C6">
+        <v>11111.1</v>
+      </c>
+      <c r="D6">
+        <f>$C6*D$5</f>
+        <v>22222.2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:L13" si="1">$C6*E$5</f>
+        <v>33333.300000000003</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>44444.4</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>55555.5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>77777.7</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>99999.900000000009</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>122222.1</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>144444.30000000002</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>188888.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="C7">
+        <v>222222.22</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D13" si="2">$C7*D$5</f>
+        <v>444444.44</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>666666.66</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>888888.88</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1111111.1000000001</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1555555.54</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1999999.98</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>2444444.42</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>2888888.86</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>3777777.74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="C8">
+        <v>3333333.3330000001</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>6666666.6660000002</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>9999999.9989999998</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>13333333.332</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>16666666.665000001</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>23333333.331</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>29999999.997000001</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>36666666.663000003</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>43333333.329000004</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>56666666.660999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+      <c r="C9">
+        <v>44444444.444399998</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>88888888.888799995</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>133333333.33319999</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>177777777.77759999</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>222222222.222</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>311111111.11079997</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>488888888.88839996</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>577777777.77719998</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>755555555.55479991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="16">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="C10" s="2">
+        <v>555555555.55554998</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>1111111111.1111</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>1666666666.6666498</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2222222222.2221999</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>2777777777.77775</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>3888888888.8888497</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>4999999999.9999495</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>6111111111.1110497</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>7222222222.2221498</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>9444444444.4443493</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6666666666.6666603</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>13333333333.333321</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>19999999999.999981</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>26666666666.666641</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>33333333333.333302</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>46666666666.666626</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>59999999999.999939</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>73333333333.333267</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>86666666666.66658</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>113333333333.33322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.74439999999999995</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>1.4887999999999999</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>2.2332000000000001</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>2.9775999999999998</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>3.7219999999999995</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>5.2107999999999999</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>6.6995999999999993</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>8.1883999999999997</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>9.6771999999999991</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>12.6548</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="C13">
+        <v>0.85555000000000003</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>1.7111000000000001</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>2.5666500000000001</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>3.4222000000000001</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>4.2777500000000002</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>5.9888500000000002</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>7.6999500000000003</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>9.4110499999999995</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>11.122150000000001</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>14.544350000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>